<commit_message>
Fixed a bug in get_loan_amount function,line loan amount input moved before the while loop
</commit_message>
<xml_diff>
--- a/docs/roadmap.xlsx
+++ b/docs/roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamasgavlider/Desktop/project 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0672095E-8C56-704D-9282-0DDBCD914AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0003D326-9B0A-494E-87A5-E2438C069DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="1280" windowWidth="23920" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>Score based on the decision is being made</t>
   </si>
   <si>
-    <t>Score - Max score 130</t>
+    <t>Score - Max score 120</t>
   </si>
 </sst>
 </file>
@@ -7558,7 +7558,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Score 30</a:t>
+            <a:t>Score 20</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -7672,7 +7672,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Score 10 </a:t>
+            <a:t>Score 0 </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -7714,7 +7714,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Score 20 </a:t>
+            <a:t>Score 10 </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -13461,7 +13461,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1800" kern="1200"/>
-            <a:t>Score 30</a:t>
+            <a:t>Score 20</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -13635,7 +13635,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1800" kern="1200"/>
-            <a:t>Score 20 </a:t>
+            <a:t>Score 10 </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -13809,7 +13809,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1800" kern="1200"/>
-            <a:t>Score 10 </a:t>
+            <a:t>Score 0 </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -29373,8 +29373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="V82" sqref="V82"/>
+    <sheetView tabSelected="1" topLeftCell="L27" workbookViewId="0">
+      <selection activeCell="AE40" sqref="AE40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add GIFs to readme
</commit_message>
<xml_diff>
--- a/docs/roadmap.xlsx
+++ b/docs/roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamasgavlider/Desktop/project 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0003D326-9B0A-494E-87A5-E2438C069DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D1FB42-5E36-814A-9A31-22C9899A2221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="1280" windowWidth="23920" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8505,42 +8505,6 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{27941B20-168E-44C7-8E13-B4FE0645B119}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>Remainder after expenses more than the monthly repayment of the loan*2 </a:t>
-          </a:r>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{586880A3-39B2-465E-9248-AD0DB9196E27}" type="parTrans" cxnId="{AFB01B68-EEB1-42EA-8E87-47B8AC602F33}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{10043882-0F71-42DA-ADCB-D2AD2D7D2496}" type="sibTrans" cxnId="{AFB01B68-EEB1-42EA-8E87-47B8AC602F33}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
     <dgm:pt modelId="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}">
       <dgm:prSet/>
       <dgm:spPr/>
@@ -8556,7 +8520,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Interes rate 0.01</a:t>
+            <a:t>Interest rate 0.01</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -8592,7 +8556,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Remainder after expenses more or equal to monthly repayment of the loan*1.5</a:t>
+            <a:t>income - expense &gt; monthly repayment of the loan*1.5</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -8670,7 +8634,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Remainder after expenses less or equal to monthly repayment of the loan</a:t>
+            <a:t>income - expense &gt;= monthly repayment of the loan</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -8739,6 +8703,121 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
+    <dgm:pt modelId="{3EE76A48-A500-9940-914A-10D6E545AD37}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>income - expense &gt; monthly repayment of the loan*2 </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DABA3FB1-AF63-1F49-B68E-9E0A2A7B28E3}" type="parTrans" cxnId="{EF61A7EB-3C7F-3F41-A273-8894686C7607}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0A2DA593-1044-F74B-9C82-0C26D768A395}" type="sibTrans" cxnId="{EF61A7EB-3C7F-3F41-A273-8894686C7607}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{99EBE0C8-EA62-0948-A203-6D622A1EBA2C}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Income - expense &lt; monthly payment</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{4E8B6560-C12A-4F48-BAFB-71F3CBAB3AEF}" type="parTrans" cxnId="{0E17A6AA-A151-074A-A1DD-C6AEF6B0F093}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DC236D27-C16D-F34F-AF03-C7773FB9D7E4}" type="sibTrans" cxnId="{0E17A6AA-A151-074A-A1DD-C6AEF6B0F093}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A99F000E-79C3-3D44-9853-563EF9AF94E8}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t>Score - 10</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t>Interest rate -.-5</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{7A2E19FA-73EA-4648-B4D7-59FAC0043BEB}" type="parTrans" cxnId="{844AF997-9E50-9C46-8E9F-EE04F2F8D95B}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{5F2B9D76-7704-A848-838E-6D900A1D0366}" type="sibTrans" cxnId="{844AF997-9E50-9C46-8E9F-EE04F2F8D95B}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
     <dgm:pt modelId="{697B2F7D-3B17-47CC-8534-20159F8BC071}" type="pres">
       <dgm:prSet presAssocID="{6DE3E276-05E4-4A56-8221-7C7D6FF303F0}" presName="Name0" presStyleCnt="0">
         <dgm:presLayoutVars>
@@ -8767,278 +8846,344 @@
       <dgm:prSet presAssocID="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" presName="level2hierChild" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{57864B81-8F04-4470-9267-28EB35714A78}" type="pres">
-      <dgm:prSet presAssocID="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{C0A3A67B-526A-4DAC-B660-74A35857F52F}" type="pres">
-      <dgm:prSet presAssocID="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{82CFD4D1-C4C7-4786-84C6-BE39E1B12815}" type="pres">
-      <dgm:prSet presAssocID="{330F8286-7B90-48F2-A754-529000A9CA9E}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{3FD72082-2FD5-45DA-A0E1-0AEFDB83D3FA}" type="pres">
-      <dgm:prSet presAssocID="{330F8286-7B90-48F2-A754-529000A9CA9E}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="4" custLinFactNeighborX="-1509">
+    <dgm:pt modelId="{91EBC5E0-9F71-7D43-BF83-38911486F0BD}" type="pres">
+      <dgm:prSet presAssocID="{4E8B6560-C12A-4F48-BAFB-71F3CBAB3AEF}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5D63D141-0A8F-2C4F-8292-EA29A4CE5794}" type="pres">
+      <dgm:prSet presAssocID="{4E8B6560-C12A-4F48-BAFB-71F3CBAB3AEF}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D63F9320-27F9-EE4C-9DAA-1268C77371A2}" type="pres">
+      <dgm:prSet presAssocID="{99EBE0C8-EA62-0948-A203-6D622A1EBA2C}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{BBE1A5C2-FD17-294F-A528-E8FBBB038CC3}" type="pres">
+      <dgm:prSet presAssocID="{99EBE0C8-EA62-0948-A203-6D622A1EBA2C}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="5">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{AB18BCAB-6B2D-4DA9-8731-1E52C97445BB}" type="pres">
-      <dgm:prSet presAssocID="{330F8286-7B90-48F2-A754-529000A9CA9E}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}" type="pres">
-      <dgm:prSet presAssocID="{046A0241-052B-469C-B88C-04DFAB629943}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{C1CBFF41-B971-4BC5-83BA-B00C9D818F9E}" type="pres">
-      <dgm:prSet presAssocID="{046A0241-052B-469C-B88C-04DFAB629943}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{FE9105A6-F49B-4266-85AC-9D28EA1DE201}" type="pres">
-      <dgm:prSet presAssocID="{28FBD105-83C6-434F-AD5C-88D40DC5F8CC}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{762E18FB-67EB-41E4-8EBC-5D3B2348F1AE}" type="pres">
-      <dgm:prSet presAssocID="{28FBD105-83C6-434F-AD5C-88D40DC5F8CC}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="4">
+    <dgm:pt modelId="{6F67DF69-A5BA-B948-BDEF-21021579FF96}" type="pres">
+      <dgm:prSet presAssocID="{99EBE0C8-EA62-0948-A203-6D622A1EBA2C}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F5B07602-6216-104D-881E-C22D3FD7B48A}" type="pres">
+      <dgm:prSet presAssocID="{7A2E19FA-73EA-4648-B4D7-59FAC0043BEB}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D6A6ED9B-6B50-484F-BBBA-EFFA339A059F}" type="pres">
+      <dgm:prSet presAssocID="{7A2E19FA-73EA-4648-B4D7-59FAC0043BEB}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{19301CE2-8805-DF4D-9E23-357E095DAA5E}" type="pres">
+      <dgm:prSet presAssocID="{A99F000E-79C3-3D44-9853-563EF9AF94E8}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{4F8902AC-2B83-1046-AEA2-477D6C7D476B}" type="pres">
+      <dgm:prSet presAssocID="{A99F000E-79C3-3D44-9853-563EF9AF94E8}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="5">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{1584BFAA-CBF9-44DD-8085-7BFFFD40F153}" type="pres">
-      <dgm:prSet presAssocID="{28FBD105-83C6-434F-AD5C-88D40DC5F8CC}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{DEDE2411-A30D-4A55-809B-43C5A22D7862}" type="pres">
-      <dgm:prSet presAssocID="{586880A3-39B2-465E-9248-AD0DB9196E27}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{23BADF63-0D80-48F5-9F10-9937578C408A}" type="pres">
-      <dgm:prSet presAssocID="{586880A3-39B2-465E-9248-AD0DB9196E27}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{853725CC-BA84-4F85-8EB2-8E0B573E191E}" type="pres">
-      <dgm:prSet presAssocID="{27941B20-168E-44C7-8E13-B4FE0645B119}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{59A5A8BE-646D-4A35-AB72-C89F408C38C1}" type="pres">
-      <dgm:prSet presAssocID="{27941B20-168E-44C7-8E13-B4FE0645B119}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="1" presStyleCnt="4">
+    <dgm:pt modelId="{6B5AD2F8-3189-D24E-8B01-3F4CD69F6F10}" type="pres">
+      <dgm:prSet presAssocID="{A99F000E-79C3-3D44-9853-563EF9AF94E8}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{57864B81-8F04-4470-9267-28EB35714A78}" type="pres">
+      <dgm:prSet presAssocID="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C0A3A67B-526A-4DAC-B660-74A35857F52F}" type="pres">
+      <dgm:prSet presAssocID="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{82CFD4D1-C4C7-4786-84C6-BE39E1B12815}" type="pres">
+      <dgm:prSet presAssocID="{330F8286-7B90-48F2-A754-529000A9CA9E}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{3FD72082-2FD5-45DA-A0E1-0AEFDB83D3FA}" type="pres">
+      <dgm:prSet presAssocID="{330F8286-7B90-48F2-A754-529000A9CA9E}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="1" presStyleCnt="5" custLinFactNeighborX="-1509">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{292E2C95-3057-43A6-8EA2-B3D4C781C9DE}" type="pres">
-      <dgm:prSet presAssocID="{27941B20-168E-44C7-8E13-B4FE0645B119}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{7BE09262-5205-4BA1-8F1F-55ACC71B1C56}" type="pres">
-      <dgm:prSet presAssocID="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{BD75137D-265A-40B5-8DC2-5F5157D13396}" type="pres">
-      <dgm:prSet presAssocID="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{03BB1352-F724-4AC7-8738-84B2B068BEBE}" type="pres">
-      <dgm:prSet presAssocID="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{095E95D6-0B9B-4DD2-B0A7-02C8F3D83AEE}" type="pres">
-      <dgm:prSet presAssocID="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="4">
+    <dgm:pt modelId="{AB18BCAB-6B2D-4DA9-8731-1E52C97445BB}" type="pres">
+      <dgm:prSet presAssocID="{330F8286-7B90-48F2-A754-529000A9CA9E}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}" type="pres">
+      <dgm:prSet presAssocID="{046A0241-052B-469C-B88C-04DFAB629943}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C1CBFF41-B971-4BC5-83BA-B00C9D818F9E}" type="pres">
+      <dgm:prSet presAssocID="{046A0241-052B-469C-B88C-04DFAB629943}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{FE9105A6-F49B-4266-85AC-9D28EA1DE201}" type="pres">
+      <dgm:prSet presAssocID="{28FBD105-83C6-434F-AD5C-88D40DC5F8CC}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{762E18FB-67EB-41E4-8EBC-5D3B2348F1AE}" type="pres">
+      <dgm:prSet presAssocID="{28FBD105-83C6-434F-AD5C-88D40DC5F8CC}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="5">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{833E4860-5898-4665-BA48-24E69197CD55}" type="pres">
-      <dgm:prSet presAssocID="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F60EF4BE-E262-410F-8D97-2339F1312225}" type="pres">
-      <dgm:prSet presAssocID="{714C6669-BDB5-424E-ACF9-91691A528875}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{9953B8B2-B267-4D6D-90D2-21032A75704D}" type="pres">
-      <dgm:prSet presAssocID="{714C6669-BDB5-424E-ACF9-91691A528875}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{CF8B8DB8-26CA-4C21-92DC-F34A05C7C1FC}" type="pres">
-      <dgm:prSet presAssocID="{37FD715F-FF73-4039-B745-FB51F8C86904}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{606CCE1F-A7DB-4848-9758-D76A1652749D}" type="pres">
-      <dgm:prSet presAssocID="{37FD715F-FF73-4039-B745-FB51F8C86904}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="4">
+    <dgm:pt modelId="{1584BFAA-CBF9-44DD-8085-7BFFFD40F153}" type="pres">
+      <dgm:prSet presAssocID="{28FBD105-83C6-434F-AD5C-88D40DC5F8CC}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{45E60197-1614-F24B-9940-ADF896B04C94}" type="pres">
+      <dgm:prSet presAssocID="{DABA3FB1-AF63-1F49-B68E-9E0A2A7B28E3}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C1B066D1-3C5A-FF4E-ABC9-77128FDF27B7}" type="pres">
+      <dgm:prSet presAssocID="{DABA3FB1-AF63-1F49-B68E-9E0A2A7B28E3}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5A7D9BA1-7D67-D747-9E3F-1B2D59CD0988}" type="pres">
+      <dgm:prSet presAssocID="{3EE76A48-A500-9940-914A-10D6E545AD37}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{370868FA-82A6-F84C-B5AC-0762E5864E9B}" type="pres">
+      <dgm:prSet presAssocID="{3EE76A48-A500-9940-914A-10D6E545AD37}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="5">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{8301E542-23AB-43B4-85D8-8A03096B5F90}" type="pres">
-      <dgm:prSet presAssocID="{37FD715F-FF73-4039-B745-FB51F8C86904}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{584ACE3F-ACE1-4261-AE80-2CB0DB735E28}" type="pres">
-      <dgm:prSet presAssocID="{F8131D2D-666B-4844-A87F-B1E037B631F3}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{00EACEB3-8021-4A5E-8ABB-273DDBE850FC}" type="pres">
-      <dgm:prSet presAssocID="{F8131D2D-666B-4844-A87F-B1E037B631F3}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{97C21B9B-2790-4E8A-8E05-8EF377213D3E}" type="pres">
-      <dgm:prSet presAssocID="{F592C52C-9D3F-4387-85D0-76C7252CB3CE}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{996D80AD-81CA-4696-85B7-0E13A7FFDEC7}" type="pres">
-      <dgm:prSet presAssocID="{F592C52C-9D3F-4387-85D0-76C7252CB3CE}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="4">
+    <dgm:pt modelId="{0FB76C49-68D0-8848-A1DD-EB3BF77732A1}" type="pres">
+      <dgm:prSet presAssocID="{3EE76A48-A500-9940-914A-10D6E545AD37}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B90C310D-D549-524B-987B-D38E9BFADBD2}" type="pres">
+      <dgm:prSet presAssocID="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{FB1D1690-90C3-EF4B-ABF0-A7868E391C19}" type="pres">
+      <dgm:prSet presAssocID="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{EFDAC0B0-541A-0847-8182-293520420773}" type="pres">
+      <dgm:prSet presAssocID="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8AB46E28-35C3-7C44-919A-064D9B12A93B}" type="pres">
+      <dgm:prSet presAssocID="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="5">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{1488A609-843B-42FC-9868-F1C4729902E2}" type="pres">
-      <dgm:prSet presAssocID="{F592C52C-9D3F-4387-85D0-76C7252CB3CE}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{77676E43-8DE8-4B80-A2D5-144E37F4A310}" type="pres">
-      <dgm:prSet presAssocID="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{3A9AC281-7E04-4189-AEA2-1A53E514D227}" type="pres">
-      <dgm:prSet presAssocID="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{6D901052-2EBD-4038-A30A-B55CA655ED9E}" type="pres">
-      <dgm:prSet presAssocID="{22C40230-3484-486B-87D8-7190AEEC3AD6}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{E82C79BE-4890-4781-B4F6-B9DDEEBD6944}" type="pres">
-      <dgm:prSet presAssocID="{22C40230-3484-486B-87D8-7190AEEC3AD6}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="4">
+    <dgm:pt modelId="{A4376C37-AE02-3F4D-BBF2-9E89618CA99C}" type="pres">
+      <dgm:prSet presAssocID="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F60EF4BE-E262-410F-8D97-2339F1312225}" type="pres">
+      <dgm:prSet presAssocID="{714C6669-BDB5-424E-ACF9-91691A528875}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9953B8B2-B267-4D6D-90D2-21032A75704D}" type="pres">
+      <dgm:prSet presAssocID="{714C6669-BDB5-424E-ACF9-91691A528875}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{CF8B8DB8-26CA-4C21-92DC-F34A05C7C1FC}" type="pres">
+      <dgm:prSet presAssocID="{37FD715F-FF73-4039-B745-FB51F8C86904}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{606CCE1F-A7DB-4848-9758-D76A1652749D}" type="pres">
+      <dgm:prSet presAssocID="{37FD715F-FF73-4039-B745-FB51F8C86904}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="5">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{58C28450-B20A-454D-AD9F-C1E26398A648}" type="pres">
-      <dgm:prSet presAssocID="{22C40230-3484-486B-87D8-7190AEEC3AD6}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{5F9E5E18-8DED-491A-B61A-67E36F30ED91}" type="pres">
-      <dgm:prSet presAssocID="{B32F3E69-C43A-48BB-ACF0-9A8FF20FEF90}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{58B11A82-8E48-4041-AD42-31A5845432BE}" type="pres">
-      <dgm:prSet presAssocID="{B32F3E69-C43A-48BB-ACF0-9A8FF20FEF90}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{63EFAE04-0ECA-4325-BBAD-BA71CD2C7ADC}" type="pres">
-      <dgm:prSet presAssocID="{510D45A9-FF5D-47C3-AF25-AD9018E18E01}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{43EC8F67-419F-4097-95A1-42F22F604BF1}" type="pres">
-      <dgm:prSet presAssocID="{510D45A9-FF5D-47C3-AF25-AD9018E18E01}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="4">
+    <dgm:pt modelId="{8301E542-23AB-43B4-85D8-8A03096B5F90}" type="pres">
+      <dgm:prSet presAssocID="{37FD715F-FF73-4039-B745-FB51F8C86904}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{584ACE3F-ACE1-4261-AE80-2CB0DB735E28}" type="pres">
+      <dgm:prSet presAssocID="{F8131D2D-666B-4844-A87F-B1E037B631F3}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{00EACEB3-8021-4A5E-8ABB-273DDBE850FC}" type="pres">
+      <dgm:prSet presAssocID="{F8131D2D-666B-4844-A87F-B1E037B631F3}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{97C21B9B-2790-4E8A-8E05-8EF377213D3E}" type="pres">
+      <dgm:prSet presAssocID="{F592C52C-9D3F-4387-85D0-76C7252CB3CE}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{996D80AD-81CA-4696-85B7-0E13A7FFDEC7}" type="pres">
+      <dgm:prSet presAssocID="{F592C52C-9D3F-4387-85D0-76C7252CB3CE}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="5">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
+    <dgm:pt modelId="{1488A609-843B-42FC-9868-F1C4729902E2}" type="pres">
+      <dgm:prSet presAssocID="{F592C52C-9D3F-4387-85D0-76C7252CB3CE}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{77676E43-8DE8-4B80-A2D5-144E37F4A310}" type="pres">
+      <dgm:prSet presAssocID="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{3A9AC281-7E04-4189-AEA2-1A53E514D227}" type="pres">
+      <dgm:prSet presAssocID="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{6D901052-2EBD-4038-A30A-B55CA655ED9E}" type="pres">
+      <dgm:prSet presAssocID="{22C40230-3484-486B-87D8-7190AEEC3AD6}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E82C79BE-4890-4781-B4F6-B9DDEEBD6944}" type="pres">
+      <dgm:prSet presAssocID="{22C40230-3484-486B-87D8-7190AEEC3AD6}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="4" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{58C28450-B20A-454D-AD9F-C1E26398A648}" type="pres">
+      <dgm:prSet presAssocID="{22C40230-3484-486B-87D8-7190AEEC3AD6}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5F9E5E18-8DED-491A-B61A-67E36F30ED91}" type="pres">
+      <dgm:prSet presAssocID="{B32F3E69-C43A-48BB-ACF0-9A8FF20FEF90}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{58B11A82-8E48-4041-AD42-31A5845432BE}" type="pres">
+      <dgm:prSet presAssocID="{B32F3E69-C43A-48BB-ACF0-9A8FF20FEF90}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{63EFAE04-0ECA-4325-BBAD-BA71CD2C7ADC}" type="pres">
+      <dgm:prSet presAssocID="{510D45A9-FF5D-47C3-AF25-AD9018E18E01}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{43EC8F67-419F-4097-95A1-42F22F604BF1}" type="pres">
+      <dgm:prSet presAssocID="{510D45A9-FF5D-47C3-AF25-AD9018E18E01}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
     <dgm:pt modelId="{752E2880-CA62-4B17-81E9-C8D585050104}" type="pres">
       <dgm:prSet presAssocID="{510D45A9-FF5D-47C3-AF25-AD9018E18E01}" presName="level3hierChild" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{A30A7A0C-FC87-6E4A-AAEF-01A6BC25DC14}" type="presOf" srcId="{4E8B6560-C12A-4F48-BAFB-71F3CBAB3AEF}" destId="{5D63D141-0A8F-2C4F-8292-EA29A4CE5794}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
     <dgm:cxn modelId="{B88C0312-ECCC-4247-8B74-45DB45237884}" srcId="{330F8286-7B90-48F2-A754-529000A9CA9E}" destId="{28FBD105-83C6-434F-AD5C-88D40DC5F8CC}" srcOrd="0" destOrd="0" parTransId="{046A0241-052B-469C-B88C-04DFAB629943}" sibTransId="{5522E76E-52C9-411C-82EB-38BFD2CAC192}"/>
-    <dgm:cxn modelId="{C846E514-8721-4C53-BFAF-5D73AA5F2145}" type="presOf" srcId="{F8131D2D-666B-4844-A87F-B1E037B631F3}" destId="{00EACEB3-8021-4A5E-8ABB-273DDBE850FC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{F2C8712E-5B20-482A-9C74-DA390984B5B8}" type="presOf" srcId="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" destId="{77676E43-8DE8-4B80-A2D5-144E37F4A310}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{A69AAB2E-0093-4E64-BAE5-7CA4281A79DB}" type="presOf" srcId="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" destId="{BD75137D-265A-40B5-8DC2-5F5157D13396}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{CAD8C92E-92C0-47DF-853F-C0AE2482733C}" type="presOf" srcId="{586880A3-39B2-465E-9248-AD0DB9196E27}" destId="{DEDE2411-A30D-4A55-809B-43C5A22D7862}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{9243F02E-7334-4E0A-B3DD-25EED5DD7F4A}" type="presOf" srcId="{37FD715F-FF73-4039-B745-FB51F8C86904}" destId="{606CCE1F-A7DB-4848-9758-D76A1652749D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{C3678C30-4D03-4652-A627-D01178D337E9}" type="presOf" srcId="{330F8286-7B90-48F2-A754-529000A9CA9E}" destId="{3FD72082-2FD5-45DA-A0E1-0AEFDB83D3FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{6B0BA535-BF4D-4934-88D6-441DBE0CE27F}" type="presOf" srcId="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" destId="{095E95D6-0B9B-4DD2-B0A7-02C8F3D83AEE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{E3836328-487F-C04F-9426-7FBF16E85C0F}" type="presOf" srcId="{99EBE0C8-EA62-0948-A203-6D622A1EBA2C}" destId="{BBE1A5C2-FD17-294F-A528-E8FBBB038CC3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{E2F8CD2D-B86E-F844-974E-9804BCE8C907}" type="presOf" srcId="{A99F000E-79C3-3D44-9853-563EF9AF94E8}" destId="{4F8902AC-2B83-1046-AEA2-477D6C7D476B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{9F2D7031-8D29-854D-BA23-4B5BE8449A7D}" type="presOf" srcId="{330F8286-7B90-48F2-A754-529000A9CA9E}" destId="{3FD72082-2FD5-45DA-A0E1-0AEFDB83D3FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{0C220437-9DDA-3D4E-90A6-D8580252D576}" type="presOf" srcId="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" destId="{3A9AC281-7E04-4189-AEA2-1A53E514D227}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{B3B5F839-5312-624A-8167-D43012DB642E}" type="presOf" srcId="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" destId="{77676E43-8DE8-4B80-A2D5-144E37F4A310}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{357F7443-FCEC-014D-BAB4-3FB99344D0D3}" type="presOf" srcId="{714C6669-BDB5-424E-ACF9-91691A528875}" destId="{F60EF4BE-E262-410F-8D97-2339F1312225}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
     <dgm:cxn modelId="{6AFFF546-B27E-49A2-93B9-270F5F17E85E}" type="presOf" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{AD3CFF9F-AEA2-4310-ADA7-A0F0768158A7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{91504B4F-F7F9-4CC4-A6A4-096483E181BF}" type="presOf" srcId="{B32F3E69-C43A-48BB-ACF0-9A8FF20FEF90}" destId="{5F9E5E18-8DED-491A-B61A-67E36F30ED91}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{35086855-5DD7-4F65-B549-751718FB08F0}" type="presOf" srcId="{046A0241-052B-469C-B88C-04DFAB629943}" destId="{C1CBFF41-B971-4BC5-83BA-B00C9D818F9E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{32C49F55-3B43-4664-9C57-44AB1B5325E9}" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{37FD715F-FF73-4039-B745-FB51F8C86904}" srcOrd="2" destOrd="0" parTransId="{714C6669-BDB5-424E-ACF9-91691A528875}" sibTransId="{EA7ACADC-91F9-453B-93AA-2997195CBDA9}"/>
-    <dgm:cxn modelId="{EBCA3F66-CBF5-4931-9FD3-FA779DB164A7}" srcId="{27941B20-168E-44C7-8E13-B4FE0645B119}" destId="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" srcOrd="0" destOrd="0" parTransId="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" sibTransId="{4E5369CC-5874-4D48-8B74-D63B06F6A177}"/>
-    <dgm:cxn modelId="{AFB01B68-EEB1-42EA-8E87-47B8AC602F33}" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{27941B20-168E-44C7-8E13-B4FE0645B119}" srcOrd="1" destOrd="0" parTransId="{586880A3-39B2-465E-9248-AD0DB9196E27}" sibTransId="{10043882-0F71-42DA-ADCB-D2AD2D7D2496}"/>
+    <dgm:cxn modelId="{A81A1B49-3E73-6C49-8DCD-7FD8BD5869B9}" type="presOf" srcId="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" destId="{8AB46E28-35C3-7C44-919A-064D9B12A93B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{4D026A4E-629A-1B40-8180-2EFF5226502B}" type="presOf" srcId="{F8131D2D-666B-4844-A87F-B1E037B631F3}" destId="{00EACEB3-8021-4A5E-8ABB-273DDBE850FC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{32C49F55-3B43-4664-9C57-44AB1B5325E9}" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{37FD715F-FF73-4039-B745-FB51F8C86904}" srcOrd="3" destOrd="0" parTransId="{714C6669-BDB5-424E-ACF9-91691A528875}" sibTransId="{EA7ACADC-91F9-453B-93AA-2997195CBDA9}"/>
+    <dgm:cxn modelId="{0E3DFF57-7629-054D-B5AA-5E503A55AA25}" type="presOf" srcId="{B32F3E69-C43A-48BB-ACF0-9A8FF20FEF90}" destId="{5F9E5E18-8DED-491A-B61A-67E36F30ED91}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{6FC6245D-7A1A-0844-A507-F24EED8A2E7D}" type="presOf" srcId="{4E8B6560-C12A-4F48-BAFB-71F3CBAB3AEF}" destId="{91EBC5E0-9F71-7D43-BF83-38911486F0BD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{7E3C9560-0713-7746-ABB3-8DD32658DC1B}" type="presOf" srcId="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" destId="{B90C310D-D549-524B-987B-D38E9BFADBD2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{C764C361-F416-A942-9715-A35C75480D0B}" type="presOf" srcId="{F8131D2D-666B-4844-A87F-B1E037B631F3}" destId="{584ACE3F-ACE1-4261-AE80-2CB0DB735E28}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{E059D661-445E-DB47-97D9-9C79A856B555}" type="presOf" srcId="{3EE76A48-A500-9940-914A-10D6E545AD37}" destId="{370868FA-82A6-F84C-B5AC-0762E5864E9B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{EBCA3F66-CBF5-4931-9FD3-FA779DB164A7}" srcId="{3EE76A48-A500-9940-914A-10D6E545AD37}" destId="{BC7D1279-1E59-4E62-A076-2D21FFFA165A}" srcOrd="0" destOrd="0" parTransId="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" sibTransId="{4E5369CC-5874-4D48-8B74-D63B06F6A177}"/>
+    <dgm:cxn modelId="{1B076F6C-23F7-F449-8E2F-9C925B614FB4}" type="presOf" srcId="{22C40230-3484-486B-87D8-7190AEEC3AD6}" destId="{E82C79BE-4890-4781-B4F6-B9DDEEBD6944}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
     <dgm:cxn modelId="{4C80E675-37D6-49F2-A792-6C3F7E02CDF6}" srcId="{37FD715F-FF73-4039-B745-FB51F8C86904}" destId="{F592C52C-9D3F-4387-85D0-76C7252CB3CE}" srcOrd="0" destOrd="0" parTransId="{F8131D2D-666B-4844-A87F-B1E037B631F3}" sibTransId="{364B5BDE-6B09-4308-AAE5-869AA063AB8D}"/>
-    <dgm:cxn modelId="{E526FB7D-8435-4CCD-BCD2-B51A40196E57}" type="presOf" srcId="{046A0241-052B-469C-B88C-04DFAB629943}" destId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{09F82C86-13F7-45AD-AE6B-E4EA2B5200A4}" type="presOf" srcId="{27941B20-168E-44C7-8E13-B4FE0645B119}" destId="{59A5A8BE-646D-4A35-AB72-C89F408C38C1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{A75CB98A-C19A-4381-927F-B8B0B32F28C4}" type="presOf" srcId="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" destId="{57864B81-8F04-4470-9267-28EB35714A78}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{7E476C8B-91C2-4325-941D-D497A14A6C1A}" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{22C40230-3484-486B-87D8-7190AEEC3AD6}" srcOrd="3" destOrd="0" parTransId="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" sibTransId="{8469BE5A-B072-4B38-BB7F-F87EF5AD408B}"/>
-    <dgm:cxn modelId="{5A39148E-2DCB-4D3B-BECC-BDA0ECD1CE38}" type="presOf" srcId="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" destId="{C0A3A67B-526A-4DAC-B660-74A35857F52F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{1D7FC37B-4295-EA4B-8EC5-21AA61220988}" type="presOf" srcId="{7A2E19FA-73EA-4648-B4D7-59FAC0043BEB}" destId="{F5B07602-6216-104D-881E-C22D3FD7B48A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{CF8A2F81-D80B-544E-926A-6A3B0FD63DCA}" type="presOf" srcId="{F592C52C-9D3F-4387-85D0-76C7252CB3CE}" destId="{996D80AD-81CA-4696-85B7-0E13A7FFDEC7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{138B8386-4EC2-8C46-B2DC-7B0596008FBB}" type="presOf" srcId="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" destId="{57864B81-8F04-4470-9267-28EB35714A78}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{7E476C8B-91C2-4325-941D-D497A14A6C1A}" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{22C40230-3484-486B-87D8-7190AEEC3AD6}" srcOrd="4" destOrd="0" parTransId="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" sibTransId="{8469BE5A-B072-4B38-BB7F-F87EF5AD408B}"/>
+    <dgm:cxn modelId="{844AF997-9E50-9C46-8E9F-EE04F2F8D95B}" srcId="{99EBE0C8-EA62-0948-A203-6D622A1EBA2C}" destId="{A99F000E-79C3-3D44-9853-563EF9AF94E8}" srcOrd="0" destOrd="0" parTransId="{7A2E19FA-73EA-4648-B4D7-59FAC0043BEB}" sibTransId="{5F2B9D76-7704-A848-838E-6D900A1D0366}"/>
+    <dgm:cxn modelId="{15D70898-FEBB-0242-AA7A-0F78B43D3781}" type="presOf" srcId="{046A0241-052B-469C-B88C-04DFAB629943}" destId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
     <dgm:cxn modelId="{1D994CA2-306A-4861-87EC-C057256E2F9F}" srcId="{22C40230-3484-486B-87D8-7190AEEC3AD6}" destId="{510D45A9-FF5D-47C3-AF25-AD9018E18E01}" srcOrd="0" destOrd="0" parTransId="{B32F3E69-C43A-48BB-ACF0-9A8FF20FEF90}" sibTransId="{22A0536A-DE8D-40F2-B3CB-6F7F9404207D}"/>
     <dgm:cxn modelId="{FDDAAFA4-9C00-457F-80D7-DC05745EDA7C}" type="presOf" srcId="{6DE3E276-05E4-4A56-8221-7C7D6FF303F0}" destId="{697B2F7D-3B17-47CC-8534-20159F8BC071}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{08B765A9-6C62-4236-862C-E52851E31A2E}" type="presOf" srcId="{510D45A9-FF5D-47C3-AF25-AD9018E18E01}" destId="{43EC8F67-419F-4097-95A1-42F22F604BF1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{6FBF51AF-8147-4CA6-89F0-C2917DBF735B}" type="presOf" srcId="{5B46684D-76C6-4DBF-BC20-3FDFCB12A6C1}" destId="{3A9AC281-7E04-4189-AEA2-1A53E514D227}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{CFBC1DC1-113C-4209-AA3A-30BE8E5D2238}" type="presOf" srcId="{F8131D2D-666B-4844-A87F-B1E037B631F3}" destId="{584ACE3F-ACE1-4261-AE80-2CB0DB735E28}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{2EDA5ECD-0356-4AF7-BCBA-6BF98C7F8DED}" type="presOf" srcId="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" destId="{7BE09262-5205-4BA1-8F1F-55ACC71B1C56}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{F1B797D7-DFE5-47BC-B84E-9DD0220DABEB}" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{330F8286-7B90-48F2-A754-529000A9CA9E}" srcOrd="0" destOrd="0" parTransId="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" sibTransId="{8F4F8D2E-3BA3-4430-9E44-4D516BAC9100}"/>
-    <dgm:cxn modelId="{C50B9BE6-6D56-46CD-A6AC-E03EE4FC0154}" type="presOf" srcId="{F592C52C-9D3F-4387-85D0-76C7252CB3CE}" destId="{996D80AD-81CA-4696-85B7-0E13A7FFDEC7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{4E8B17E7-45F4-4F81-A52B-493585732421}" type="presOf" srcId="{714C6669-BDB5-424E-ACF9-91691A528875}" destId="{F60EF4BE-E262-410F-8D97-2339F1312225}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{208566E9-AB8F-4AE8-A441-E56126DD939B}" type="presOf" srcId="{586880A3-39B2-465E-9248-AD0DB9196E27}" destId="{23BADF63-0D80-48F5-9F10-9937578C408A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{CFB23DF1-284A-4F4C-BC63-36CCFB9BE9A4}" type="presOf" srcId="{B32F3E69-C43A-48BB-ACF0-9A8FF20FEF90}" destId="{58B11A82-8E48-4041-AD42-31A5845432BE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{0E17A6AA-A151-074A-A1DD-C6AEF6B0F093}" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{99EBE0C8-EA62-0948-A203-6D622A1EBA2C}" srcOrd="0" destOrd="0" parTransId="{4E8B6560-C12A-4F48-BAFB-71F3CBAB3AEF}" sibTransId="{DC236D27-C16D-F34F-AF03-C7773FB9D7E4}"/>
+    <dgm:cxn modelId="{3466EFB4-833F-A242-9908-E417CE9CB641}" type="presOf" srcId="{046A0241-052B-469C-B88C-04DFAB629943}" destId="{C1CBFF41-B971-4BC5-83BA-B00C9D818F9E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{7A5803BA-E73D-F44A-B572-64D357EE557B}" type="presOf" srcId="{28FBD105-83C6-434F-AD5C-88D40DC5F8CC}" destId="{762E18FB-67EB-41E4-8EBC-5D3B2348F1AE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{6AA694C5-11FC-CD47-9FC2-8A0EDDF3CB79}" type="presOf" srcId="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" destId="{C0A3A67B-526A-4DAC-B660-74A35857F52F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{13BA08D5-D91D-3446-B491-1A305F7AD512}" type="presOf" srcId="{510D45A9-FF5D-47C3-AF25-AD9018E18E01}" destId="{43EC8F67-419F-4097-95A1-42F22F604BF1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{F1B797D7-DFE5-47BC-B84E-9DD0220DABEB}" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{330F8286-7B90-48F2-A754-529000A9CA9E}" srcOrd="1" destOrd="0" parTransId="{0CD30D3E-AAA5-42F4-A520-C2094DE42880}" sibTransId="{8F4F8D2E-3BA3-4430-9E44-4D516BAC9100}"/>
+    <dgm:cxn modelId="{B251DBD8-E4C2-9D40-BF6C-C734E6F08FBB}" type="presOf" srcId="{DABA3FB1-AF63-1F49-B68E-9E0A2A7B28E3}" destId="{45E60197-1614-F24B-9940-ADF896B04C94}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{8DDECCDE-D4EE-8345-BA0F-CCB6F219D703}" type="presOf" srcId="{B32F3E69-C43A-48BB-ACF0-9A8FF20FEF90}" destId="{58B11A82-8E48-4041-AD42-31A5845432BE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{EF61A7EB-3C7F-3F41-A273-8894686C7607}" srcId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" destId="{3EE76A48-A500-9940-914A-10D6E545AD37}" srcOrd="2" destOrd="0" parTransId="{DABA3FB1-AF63-1F49-B68E-9E0A2A7B28E3}" sibTransId="{0A2DA593-1044-F74B-9C82-0C26D768A395}"/>
+    <dgm:cxn modelId="{0D7EEDEE-417D-964B-B94C-B6913955EE57}" type="presOf" srcId="{7A2E19FA-73EA-4648-B4D7-59FAC0043BEB}" destId="{D6A6ED9B-6B50-484F-BBBA-EFFA339A059F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{F35382F0-A128-8B44-A946-679975064740}" type="presOf" srcId="{DABA3FB1-AF63-1F49-B68E-9E0A2A7B28E3}" destId="{C1B066D1-3C5A-FF4E-ABC9-77128FDF27B7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
     <dgm:cxn modelId="{20E697F3-F46B-4718-A698-442579D72CFB}" srcId="{6DE3E276-05E4-4A56-8221-7C7D6FF303F0}" destId="{62C7E9BE-0B2A-4FBC-A770-A96BF79B3D91}" srcOrd="0" destOrd="0" parTransId="{B792632A-AA47-41E3-9F37-BC0A54A1BD08}" sibTransId="{C1DD3EE1-E0AF-49B4-B9B9-D284F1DCDB21}"/>
-    <dgm:cxn modelId="{C8DCC0F5-B662-45B3-B10A-A6133C79B0A4}" type="presOf" srcId="{22C40230-3484-486B-87D8-7190AEEC3AD6}" destId="{E82C79BE-4890-4781-B4F6-B9DDEEBD6944}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{3EFD19FA-69B9-4031-B82D-27A064351D01}" type="presOf" srcId="{28FBD105-83C6-434F-AD5C-88D40DC5F8CC}" destId="{762E18FB-67EB-41E4-8EBC-5D3B2348F1AE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{BA0F87FA-E00A-4E12-A7B5-97B5F3EA5EFF}" type="presOf" srcId="{714C6669-BDB5-424E-ACF9-91691A528875}" destId="{9953B8B2-B267-4D6D-90D2-21032A75704D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{40C812F6-6865-E949-8020-9598C6B9A6B2}" type="presOf" srcId="{C4DCF0E4-B0BA-4FEA-BDD8-8CA0553FC6E3}" destId="{FB1D1690-90C3-EF4B-ABF0-A7868E391C19}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{D9E3BAFC-58CC-B44F-BCC9-152CE4C2D9F5}" type="presOf" srcId="{714C6669-BDB5-424E-ACF9-91691A528875}" destId="{9953B8B2-B267-4D6D-90D2-21032A75704D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{1619F1FE-1FFE-1842-B0D5-8D39D43BFC1D}" type="presOf" srcId="{37FD715F-FF73-4039-B745-FB51F8C86904}" destId="{606CCE1F-A7DB-4848-9758-D76A1652749D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
     <dgm:cxn modelId="{1DB14A5B-785E-4D41-A6E3-2BCDDE36211B}" type="presParOf" srcId="{697B2F7D-3B17-47CC-8534-20159F8BC071}" destId="{B503D9DE-E208-42C2-A97B-088433B18A5E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
     <dgm:cxn modelId="{5C963F53-C26C-44FC-B9FE-F0B57E8AD771}" type="presParOf" srcId="{B503D9DE-E208-42C2-A97B-088433B18A5E}" destId="{AD3CFF9F-AEA2-4310-ADA7-A0F0768158A7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
     <dgm:cxn modelId="{2B541445-A097-42B3-A483-8E73B53F01BD}" type="presParOf" srcId="{B503D9DE-E208-42C2-A97B-088433B18A5E}" destId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{A366C7EC-7D8B-4D00-BA78-459998DC443B}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{57864B81-8F04-4470-9267-28EB35714A78}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{9EFAB0A4-F394-4F82-9B1E-7867BFB47619}" type="presParOf" srcId="{57864B81-8F04-4470-9267-28EB35714A78}" destId="{C0A3A67B-526A-4DAC-B660-74A35857F52F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{5A2492FB-96BB-4F08-8951-083DCA092CA7}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{82CFD4D1-C4C7-4786-84C6-BE39E1B12815}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{43E721A0-872E-4304-9322-9B016D6B95D3}" type="presParOf" srcId="{82CFD4D1-C4C7-4786-84C6-BE39E1B12815}" destId="{3FD72082-2FD5-45DA-A0E1-0AEFDB83D3FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{FC10C011-EDCD-4F5C-8B27-A546A0F85DB9}" type="presParOf" srcId="{82CFD4D1-C4C7-4786-84C6-BE39E1B12815}" destId="{AB18BCAB-6B2D-4DA9-8731-1E52C97445BB}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{B53F4E01-C06D-45B8-90E4-FC65FD2EF0B8}" type="presParOf" srcId="{AB18BCAB-6B2D-4DA9-8731-1E52C97445BB}" destId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{27C124AA-73AA-47E9-8C0E-E04E6C7D8B33}" type="presParOf" srcId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}" destId="{C1CBFF41-B971-4BC5-83BA-B00C9D818F9E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{739D1226-3E13-489C-8E78-9CAD8D1051E2}" type="presParOf" srcId="{AB18BCAB-6B2D-4DA9-8731-1E52C97445BB}" destId="{FE9105A6-F49B-4266-85AC-9D28EA1DE201}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{CEB6646B-BD7C-4892-8CF1-95F0AB376A55}" type="presParOf" srcId="{FE9105A6-F49B-4266-85AC-9D28EA1DE201}" destId="{762E18FB-67EB-41E4-8EBC-5D3B2348F1AE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{4E209784-7D04-45CB-BA8F-A031E510ACAC}" type="presParOf" srcId="{FE9105A6-F49B-4266-85AC-9D28EA1DE201}" destId="{1584BFAA-CBF9-44DD-8085-7BFFFD40F153}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{7BC7EA82-FD8F-48CA-8CFB-9DEE20902F4C}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{DEDE2411-A30D-4A55-809B-43C5A22D7862}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{235C33B8-3B22-4C14-B4E2-64BDE36A89D3}" type="presParOf" srcId="{DEDE2411-A30D-4A55-809B-43C5A22D7862}" destId="{23BADF63-0D80-48F5-9F10-9937578C408A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{91186816-CBD4-47A6-B6A3-7B343977122A}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{853725CC-BA84-4F85-8EB2-8E0B573E191E}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{D90A6F77-9AF5-40B3-AED9-95B2D6030D78}" type="presParOf" srcId="{853725CC-BA84-4F85-8EB2-8E0B573E191E}" destId="{59A5A8BE-646D-4A35-AB72-C89F408C38C1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{5732C16A-5D24-41B7-9177-C414B343B2B7}" type="presParOf" srcId="{853725CC-BA84-4F85-8EB2-8E0B573E191E}" destId="{292E2C95-3057-43A6-8EA2-B3D4C781C9DE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{70544EB6-E80A-427D-B90D-936335086F9C}" type="presParOf" srcId="{292E2C95-3057-43A6-8EA2-B3D4C781C9DE}" destId="{7BE09262-5205-4BA1-8F1F-55ACC71B1C56}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{0F7EC801-2089-494D-B518-7AF0D1DF65A9}" type="presParOf" srcId="{7BE09262-5205-4BA1-8F1F-55ACC71B1C56}" destId="{BD75137D-265A-40B5-8DC2-5F5157D13396}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{D62B367F-ADDF-42AE-B0CA-A36672A945E3}" type="presParOf" srcId="{292E2C95-3057-43A6-8EA2-B3D4C781C9DE}" destId="{03BB1352-F724-4AC7-8738-84B2B068BEBE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{F03B1EE4-3752-4CCC-83F7-90E1BD4A071F}" type="presParOf" srcId="{03BB1352-F724-4AC7-8738-84B2B068BEBE}" destId="{095E95D6-0B9B-4DD2-B0A7-02C8F3D83AEE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{4889C896-A603-4FBD-9CFE-CDB155CC2A46}" type="presParOf" srcId="{03BB1352-F724-4AC7-8738-84B2B068BEBE}" destId="{833E4860-5898-4665-BA48-24E69197CD55}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{EB1B848F-1B23-4437-A9F2-15C130F8512D}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{F60EF4BE-E262-410F-8D97-2339F1312225}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{DA928A75-81B5-4C35-BA51-0ACFB29F8E19}" type="presParOf" srcId="{F60EF4BE-E262-410F-8D97-2339F1312225}" destId="{9953B8B2-B267-4D6D-90D2-21032A75704D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{7D7998A9-C366-4947-BB3A-B80AE4ECC3B2}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{CF8B8DB8-26CA-4C21-92DC-F34A05C7C1FC}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{AE126FC6-4C29-4560-8204-D0D6CF3E4501}" type="presParOf" srcId="{CF8B8DB8-26CA-4C21-92DC-F34A05C7C1FC}" destId="{606CCE1F-A7DB-4848-9758-D76A1652749D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{D6AD29A5-3198-458F-BD46-526590A49C0C}" type="presParOf" srcId="{CF8B8DB8-26CA-4C21-92DC-F34A05C7C1FC}" destId="{8301E542-23AB-43B4-85D8-8A03096B5F90}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{F4529A09-E110-443D-B174-CE0DA5216F96}" type="presParOf" srcId="{8301E542-23AB-43B4-85D8-8A03096B5F90}" destId="{584ACE3F-ACE1-4261-AE80-2CB0DB735E28}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{B61E91F4-33B1-4CF8-860C-E040256DC8F4}" type="presParOf" srcId="{584ACE3F-ACE1-4261-AE80-2CB0DB735E28}" destId="{00EACEB3-8021-4A5E-8ABB-273DDBE850FC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{004738A6-4871-4CDA-A8C8-214F35795A6E}" type="presParOf" srcId="{8301E542-23AB-43B4-85D8-8A03096B5F90}" destId="{97C21B9B-2790-4E8A-8E05-8EF377213D3E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{8934CFFE-B4CD-4CD0-931C-866EB4273A39}" type="presParOf" srcId="{97C21B9B-2790-4E8A-8E05-8EF377213D3E}" destId="{996D80AD-81CA-4696-85B7-0E13A7FFDEC7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{38EE59CD-C383-4E06-BAFC-713C1D007AD9}" type="presParOf" srcId="{97C21B9B-2790-4E8A-8E05-8EF377213D3E}" destId="{1488A609-843B-42FC-9868-F1C4729902E2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{357A283E-64B3-4142-A4B6-12E2F558E1FA}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{77676E43-8DE8-4B80-A2D5-144E37F4A310}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{3A42CADA-23F4-4775-81E5-181403393D61}" type="presParOf" srcId="{77676E43-8DE8-4B80-A2D5-144E37F4A310}" destId="{3A9AC281-7E04-4189-AEA2-1A53E514D227}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{9E2504C8-D9DA-4597-A1C4-3DE03EDBCFDA}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{6D901052-2EBD-4038-A30A-B55CA655ED9E}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{CAD0E745-D7CA-454C-91FA-A53DB93919E8}" type="presParOf" srcId="{6D901052-2EBD-4038-A30A-B55CA655ED9E}" destId="{E82C79BE-4890-4781-B4F6-B9DDEEBD6944}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{524181B0-1DC8-4586-AA33-3266A386DB3D}" type="presParOf" srcId="{6D901052-2EBD-4038-A30A-B55CA655ED9E}" destId="{58C28450-B20A-454D-AD9F-C1E26398A648}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{3B1211C8-5C4C-4834-8716-88BB06E28768}" type="presParOf" srcId="{58C28450-B20A-454D-AD9F-C1E26398A648}" destId="{5F9E5E18-8DED-491A-B61A-67E36F30ED91}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{3498E9A3-7C8C-4290-92A3-5FCF55489BC0}" type="presParOf" srcId="{5F9E5E18-8DED-491A-B61A-67E36F30ED91}" destId="{58B11A82-8E48-4041-AD42-31A5845432BE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{5A65C874-E622-4B22-BADA-C2422BE37D37}" type="presParOf" srcId="{58C28450-B20A-454D-AD9F-C1E26398A648}" destId="{63EFAE04-0ECA-4325-BBAD-BA71CD2C7ADC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{5798EC0D-387D-43BB-8299-6D3AA58ECB0A}" type="presParOf" srcId="{63EFAE04-0ECA-4325-BBAD-BA71CD2C7ADC}" destId="{43EC8F67-419F-4097-95A1-42F22F604BF1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
-    <dgm:cxn modelId="{3AD5B259-7B2D-418B-881E-3EA4A413502B}" type="presParOf" srcId="{63EFAE04-0ECA-4325-BBAD-BA71CD2C7ADC}" destId="{752E2880-CA62-4B17-81E9-C8D585050104}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{A18DFE77-1F9B-A741-951C-4D7B8FA72454}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{91EBC5E0-9F71-7D43-BF83-38911486F0BD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{1AA6B4EA-C3EA-3B4E-A1D6-6E5030F91D9D}" type="presParOf" srcId="{91EBC5E0-9F71-7D43-BF83-38911486F0BD}" destId="{5D63D141-0A8F-2C4F-8292-EA29A4CE5794}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{D2D52157-A508-D742-B69A-286FA7E8AD35}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{D63F9320-27F9-EE4C-9DAA-1268C77371A2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{E1BE3EC1-56B1-C346-931A-3C35C2315DED}" type="presParOf" srcId="{D63F9320-27F9-EE4C-9DAA-1268C77371A2}" destId="{BBE1A5C2-FD17-294F-A528-E8FBBB038CC3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{F94B28A5-21AD-6C4B-8975-8ED3CA8F3BAE}" type="presParOf" srcId="{D63F9320-27F9-EE4C-9DAA-1268C77371A2}" destId="{6F67DF69-A5BA-B948-BDEF-21021579FF96}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{21A0BFF4-5DF1-9740-81EC-B1B126A5F4FE}" type="presParOf" srcId="{6F67DF69-A5BA-B948-BDEF-21021579FF96}" destId="{F5B07602-6216-104D-881E-C22D3FD7B48A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{7D41D28B-6D97-D941-9ED4-D5AE62B2B853}" type="presParOf" srcId="{F5B07602-6216-104D-881E-C22D3FD7B48A}" destId="{D6A6ED9B-6B50-484F-BBBA-EFFA339A059F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{751EA123-BCE9-A545-ABE4-94A6599B159B}" type="presParOf" srcId="{6F67DF69-A5BA-B948-BDEF-21021579FF96}" destId="{19301CE2-8805-DF4D-9E23-357E095DAA5E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{4AF0C58E-A73F-EA44-88BE-D7F66A281161}" type="presParOf" srcId="{19301CE2-8805-DF4D-9E23-357E095DAA5E}" destId="{4F8902AC-2B83-1046-AEA2-477D6C7D476B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{1C53F3ED-F8A2-6E48-BF90-4CAE075BA93B}" type="presParOf" srcId="{19301CE2-8805-DF4D-9E23-357E095DAA5E}" destId="{6B5AD2F8-3189-D24E-8B01-3F4CD69F6F10}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{223E98FE-484B-6849-A3D6-0341FEC518C7}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{57864B81-8F04-4470-9267-28EB35714A78}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{0D3B0F4F-B90A-FB4B-AF2A-6A49A6EF825F}" type="presParOf" srcId="{57864B81-8F04-4470-9267-28EB35714A78}" destId="{C0A3A67B-526A-4DAC-B660-74A35857F52F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{5D376E58-CF9B-204F-8A3F-96BCF1A01DD1}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{82CFD4D1-C4C7-4786-84C6-BE39E1B12815}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{7E3E75A0-B0B2-604B-9E09-C494E0ECF7C4}" type="presParOf" srcId="{82CFD4D1-C4C7-4786-84C6-BE39E1B12815}" destId="{3FD72082-2FD5-45DA-A0E1-0AEFDB83D3FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{E15D674E-FC16-6F4D-B872-5BF63EDBA128}" type="presParOf" srcId="{82CFD4D1-C4C7-4786-84C6-BE39E1B12815}" destId="{AB18BCAB-6B2D-4DA9-8731-1E52C97445BB}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{B43482AF-3B7F-534A-A33E-835EAEDEC418}" type="presParOf" srcId="{AB18BCAB-6B2D-4DA9-8731-1E52C97445BB}" destId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{7365F6DC-0742-3541-8702-091FCA7DBDBB}" type="presParOf" srcId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}" destId="{C1CBFF41-B971-4BC5-83BA-B00C9D818F9E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{27B8EDA3-3E98-3E4C-A641-5749FA1C5D57}" type="presParOf" srcId="{AB18BCAB-6B2D-4DA9-8731-1E52C97445BB}" destId="{FE9105A6-F49B-4266-85AC-9D28EA1DE201}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{42966A77-99DB-A741-B5E8-1C230EB9A9AE}" type="presParOf" srcId="{FE9105A6-F49B-4266-85AC-9D28EA1DE201}" destId="{762E18FB-67EB-41E4-8EBC-5D3B2348F1AE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{DD3FEE63-7FDB-FD40-8979-085BE256C852}" type="presParOf" srcId="{FE9105A6-F49B-4266-85AC-9D28EA1DE201}" destId="{1584BFAA-CBF9-44DD-8085-7BFFFD40F153}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{B0E5F2FB-6F47-264F-9D2D-3374235FBBB4}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{45E60197-1614-F24B-9940-ADF896B04C94}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{5BE37729-B65D-E54F-BCE4-E9FB305295A2}" type="presParOf" srcId="{45E60197-1614-F24B-9940-ADF896B04C94}" destId="{C1B066D1-3C5A-FF4E-ABC9-77128FDF27B7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{3AFF78BA-ECFA-774D-B305-881F74BA1DFB}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{5A7D9BA1-7D67-D747-9E3F-1B2D59CD0988}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{3A506495-279E-784A-BDC5-E52627AD774D}" type="presParOf" srcId="{5A7D9BA1-7D67-D747-9E3F-1B2D59CD0988}" destId="{370868FA-82A6-F84C-B5AC-0762E5864E9B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{C1BC66A2-25F3-2C4D-90EC-207E1F734887}" type="presParOf" srcId="{5A7D9BA1-7D67-D747-9E3F-1B2D59CD0988}" destId="{0FB76C49-68D0-8848-A1DD-EB3BF77732A1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{EE04F2CF-A4D1-2548-9CF8-AD76DA966125}" type="presParOf" srcId="{0FB76C49-68D0-8848-A1DD-EB3BF77732A1}" destId="{B90C310D-D549-524B-987B-D38E9BFADBD2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{34B7F413-A342-5F45-B9A0-390ED6B02F1D}" type="presParOf" srcId="{B90C310D-D549-524B-987B-D38E9BFADBD2}" destId="{FB1D1690-90C3-EF4B-ABF0-A7868E391C19}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{9FF7290B-7D14-794C-98B9-652A786E68F0}" type="presParOf" srcId="{0FB76C49-68D0-8848-A1DD-EB3BF77732A1}" destId="{EFDAC0B0-541A-0847-8182-293520420773}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{96B9AB41-56D5-B14B-B832-01EFC724D367}" type="presParOf" srcId="{EFDAC0B0-541A-0847-8182-293520420773}" destId="{8AB46E28-35C3-7C44-919A-064D9B12A93B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{895066DE-CBEF-C849-A007-7351D1DF324C}" type="presParOf" srcId="{EFDAC0B0-541A-0847-8182-293520420773}" destId="{A4376C37-AE02-3F4D-BBF2-9E89618CA99C}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{DC8CEAA0-FAE1-FA48-8977-63096228AF87}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{F60EF4BE-E262-410F-8D97-2339F1312225}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{8CFFEE33-576E-7248-8AAF-5CF7DF29F1E0}" type="presParOf" srcId="{F60EF4BE-E262-410F-8D97-2339F1312225}" destId="{9953B8B2-B267-4D6D-90D2-21032A75704D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{E366B1E6-27F3-584C-B69B-16534042635C}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{CF8B8DB8-26CA-4C21-92DC-F34A05C7C1FC}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{7FBE0BCF-B8D3-2F4F-B4A7-F18458E30FF7}" type="presParOf" srcId="{CF8B8DB8-26CA-4C21-92DC-F34A05C7C1FC}" destId="{606CCE1F-A7DB-4848-9758-D76A1652749D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{C38F1A35-9079-3543-B5D0-73C2F9A29272}" type="presParOf" srcId="{CF8B8DB8-26CA-4C21-92DC-F34A05C7C1FC}" destId="{8301E542-23AB-43B4-85D8-8A03096B5F90}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{43521037-61AB-5B41-908A-027C47A0F9DE}" type="presParOf" srcId="{8301E542-23AB-43B4-85D8-8A03096B5F90}" destId="{584ACE3F-ACE1-4261-AE80-2CB0DB735E28}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{D2494E7F-F4D4-2946-8613-94C77D93747F}" type="presParOf" srcId="{584ACE3F-ACE1-4261-AE80-2CB0DB735E28}" destId="{00EACEB3-8021-4A5E-8ABB-273DDBE850FC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{5164184D-F8E4-D64E-BFAA-BBC957D489B4}" type="presParOf" srcId="{8301E542-23AB-43B4-85D8-8A03096B5F90}" destId="{97C21B9B-2790-4E8A-8E05-8EF377213D3E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{D1D4DD34-9645-D24B-9099-BDD54FA9F804}" type="presParOf" srcId="{97C21B9B-2790-4E8A-8E05-8EF377213D3E}" destId="{996D80AD-81CA-4696-85B7-0E13A7FFDEC7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{222208DD-73BC-3646-B9F4-C81EAD0D1469}" type="presParOf" srcId="{97C21B9B-2790-4E8A-8E05-8EF377213D3E}" destId="{1488A609-843B-42FC-9868-F1C4729902E2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{CEB7DB91-D663-9348-86BD-DD06129C9D4D}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{77676E43-8DE8-4B80-A2D5-144E37F4A310}" srcOrd="8" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{B73D416D-6361-2643-B2A9-BB36946A2A25}" type="presParOf" srcId="{77676E43-8DE8-4B80-A2D5-144E37F4A310}" destId="{3A9AC281-7E04-4189-AEA2-1A53E514D227}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{C130794C-08F8-1147-A041-0815730C2930}" type="presParOf" srcId="{9C211E10-BDA4-4C4E-B560-088C5F2D42D7}" destId="{6D901052-2EBD-4038-A30A-B55CA655ED9E}" srcOrd="9" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{0AAADE42-ED70-1241-8180-CB6B3D3E3CAC}" type="presParOf" srcId="{6D901052-2EBD-4038-A30A-B55CA655ED9E}" destId="{E82C79BE-4890-4781-B4F6-B9DDEEBD6944}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{AB603A2B-884A-BE4A-AD04-57A71C701E2E}" type="presParOf" srcId="{6D901052-2EBD-4038-A30A-B55CA655ED9E}" destId="{58C28450-B20A-454D-AD9F-C1E26398A648}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{5B3B5CC8-6EBC-2645-AC3F-5123202BB2B5}" type="presParOf" srcId="{58C28450-B20A-454D-AD9F-C1E26398A648}" destId="{5F9E5E18-8DED-491A-B61A-67E36F30ED91}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{528820AD-8013-564A-936D-563E3E3DF31C}" type="presParOf" srcId="{5F9E5E18-8DED-491A-B61A-67E36F30ED91}" destId="{58B11A82-8E48-4041-AD42-31A5845432BE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{96440A4A-EA6A-1D4F-A40B-6FEE7EC1E7CD}" type="presParOf" srcId="{58C28450-B20A-454D-AD9F-C1E26398A648}" destId="{63EFAE04-0ECA-4325-BBAD-BA71CD2C7ADC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{35506BD3-043C-6F46-B477-5739B7D1D0CD}" type="presParOf" srcId="{63EFAE04-0ECA-4325-BBAD-BA71CD2C7ADC}" destId="{43EC8F67-419F-4097-95A1-42F22F604BF1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
+    <dgm:cxn modelId="{AADFA4CD-073B-0742-890E-1C2531EE3DA4}" type="presParOf" srcId="{63EFAE04-0ECA-4325-BBAD-BA71CD2C7ADC}" destId="{752E2880-CA62-4B17-81E9-C8D585050104}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/HorizontalMultiLevelHierarchy"/>
   </dgm:cxnLst>
   <dgm:bg/>
   <dgm:whole/>
@@ -9181,7 +9326,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Score -100</a:t>
+            <a:t>Score -120</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -9443,7 +9588,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" type="asst">
+    <dgm:pt modelId="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" type="asst">
       <dgm:prSet phldrT="[Text]"/>
       <dgm:spPr/>
       <dgm:t>
@@ -9452,12 +9597,12 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Between 50 - 90</a:t>
+            <a:t>Score &gt;= 70</a:t>
           </a:r>
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{2AA4CF4B-BF09-48D5-A141-23C39086599F}" type="parTrans" cxnId="{D6B8891C-5ABA-4611-AF88-E4AD84CF5053}">
+    <dgm:pt modelId="{15D2CF99-A2B9-418C-A563-4BA672D4EC74}" type="parTrans" cxnId="{A403D5CE-6600-4597-8B62-30A182D01FD5}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -9468,7 +9613,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{FA3856B3-B1DD-48FB-8F49-43F2C8D53F0D}" type="sibTrans" cxnId="{D6B8891C-5ABA-4611-AF88-E4AD84CF5053}">
+    <dgm:pt modelId="{FB661218-E898-466B-A96A-8A3EB830EA43}" type="sibTrans" cxnId="{A403D5CE-6600-4597-8B62-30A182D01FD5}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -9479,7 +9624,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" type="asst">
+    <dgm:pt modelId="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" type="asst">
       <dgm:prSet phldrT="[Text]"/>
       <dgm:spPr/>
       <dgm:t>
@@ -9488,43 +9633,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Over 90</a:t>
-          </a:r>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{15D2CF99-A2B9-418C-A563-4BA672D4EC74}" type="parTrans" cxnId="{A403D5CE-6600-4597-8B62-30A182D01FD5}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{FB661218-E898-466B-A96A-8A3EB830EA43}" type="sibTrans" cxnId="{A403D5CE-6600-4597-8B62-30A182D01FD5}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" type="asst">
-      <dgm:prSet phldrT="[Text]"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>Under 50</a:t>
+            <a:t>Score &lt; 70</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -9577,42 +9686,6 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C6335AA2-590A-4C67-86E5-3EA4B7D8771A}" type="sibTrans" cxnId="{170AEB47-9EA9-406C-A14A-63EBA18F0B60}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" type="asst">
-      <dgm:prSet phldrT="[Text]"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>Approved</a:t>
-          </a:r>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{97A0BEBB-D5A9-4338-BDDC-BB6757A5DA75}" type="parTrans" cxnId="{31CDC28C-50B9-46B8-91B6-CE93A8E85FF9}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{28F7DDC4-D7CA-4BF1-848F-D5B1B6F067CB}" type="sibTrans" cxnId="{31CDC28C-50B9-46B8-91B6-CE93A8E85FF9}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -9685,7 +9758,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{57FE20FB-F5E0-4DA2-9D76-4A2A6628A15A}" type="pres">
-      <dgm:prSet presAssocID="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" presName="rootText1" presStyleLbl="node0" presStyleIdx="0" presStyleCnt="3">
+      <dgm:prSet presAssocID="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" presName="rootText1" presStyleLbl="node0" presStyleIdx="0" presStyleCnt="2">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -9693,7 +9766,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{0B0179FF-84DE-48B2-A7B2-7647C4DEF74C}" type="pres">
-      <dgm:prSet presAssocID="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" presName="rootConnector1" presStyleLbl="asst0" presStyleIdx="0" presStyleCnt="3"/>
+      <dgm:prSet presAssocID="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" presName="rootConnector1" presStyleLbl="asst0" presStyleIdx="0" presStyleCnt="2"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{B0C93200-9340-43D6-B0E3-DE54C1489742}" type="pres">
@@ -9705,7 +9778,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{72416332-1284-4FEA-973A-34B4871CCC3F}" type="pres">
-      <dgm:prSet presAssocID="{3F3288E7-6B47-4EB6-917A-860E6A2B7D52}" presName="Name111" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="3"/>
+      <dgm:prSet presAssocID="{3F3288E7-6B47-4EB6-917A-860E6A2B7D52}" presName="Name111" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="2"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{6214A9CC-647A-4E83-9BFC-93AAA1510EFC}" type="pres">
@@ -9721,7 +9794,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{AF7FB488-574D-4E27-9A8E-92293D2D553D}" type="pres">
-      <dgm:prSet presAssocID="{9439E707-2878-455D-93F3-E63F2486DDE0}" presName="rootText3" presStyleLbl="asst0" presStyleIdx="0" presStyleCnt="3">
+      <dgm:prSet presAssocID="{9439E707-2878-455D-93F3-E63F2486DDE0}" presName="rootText3" presStyleLbl="asst0" presStyleIdx="0" presStyleCnt="2">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -9729,7 +9802,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{4B2205FC-4A1F-4EBD-AC56-8E8D946DFC3B}" type="pres">
-      <dgm:prSet presAssocID="{9439E707-2878-455D-93F3-E63F2486DDE0}" presName="rootConnector3" presStyleLbl="asst0" presStyleIdx="0" presStyleCnt="3"/>
+      <dgm:prSet presAssocID="{9439E707-2878-455D-93F3-E63F2486DDE0}" presName="rootConnector3" presStyleLbl="asst0" presStyleIdx="0" presStyleCnt="2"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{2994D162-FD3E-4980-90DB-B1833056775E}" type="pres">
@@ -9738,74 +9811,6 @@
     </dgm:pt>
     <dgm:pt modelId="{F367418B-F286-440A-9A7B-2BDEEDA71E8B}" type="pres">
       <dgm:prSet presAssocID="{9439E707-2878-455D-93F3-E63F2486DDE0}" presName="hierChild7" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{D6E38978-9D05-4C1C-BEFF-EF82F634E34B}" type="pres">
-      <dgm:prSet presAssocID="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" presName="hierRoot1" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{178DCAA2-D7AA-4AE4-8110-84AE55DAFB4C}" type="pres">
-      <dgm:prSet presAssocID="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" presName="rootComposite1" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{76AD2B5F-A78D-4688-A301-5DE4286FAF14}" type="pres">
-      <dgm:prSet presAssocID="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" presName="rootText1" presStyleLbl="node0" presStyleIdx="1" presStyleCnt="3">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{277E8B4D-5DAC-4C00-95B2-6E5ADFBAA0BC}" type="pres">
-      <dgm:prSet presAssocID="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" presName="rootConnector1" presStyleLbl="asst0" presStyleIdx="0" presStyleCnt="3"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{BC4D512F-D5D5-4EC4-AB91-99C49864A5DC}" type="pres">
-      <dgm:prSet presAssocID="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" presName="hierChild2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{8A58ACB5-52B2-4818-B571-1DE60B545CAF}" type="pres">
-      <dgm:prSet presAssocID="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" presName="hierChild3" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{758BB659-965A-451E-B239-65B733991407}" type="pres">
-      <dgm:prSet presAssocID="{97A0BEBB-D5A9-4338-BDDC-BB6757A5DA75}" presName="Name111" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="3"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{3AE659BE-DB29-4625-8029-1B3242160EB5}" type="pres">
-      <dgm:prSet presAssocID="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" presName="hierRoot3" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{3B733DE7-3A47-4186-87B5-A06E7664D23B}" type="pres">
-      <dgm:prSet presAssocID="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" presName="rootComposite3" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{843CB9D4-FFDE-40CB-BDF4-1B14FA03BEEE}" type="pres">
-      <dgm:prSet presAssocID="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" presName="rootText3" presStyleLbl="asst0" presStyleIdx="1" presStyleCnt="3">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{742B2A4B-0C31-45FA-A574-C4B63CA27F49}" type="pres">
-      <dgm:prSet presAssocID="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" presName="rootConnector3" presStyleLbl="asst0" presStyleIdx="1" presStyleCnt="3"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F3383217-A95D-4C77-B90E-4D8D3300A368}" type="pres">
-      <dgm:prSet presAssocID="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" presName="hierChild6" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{473CAF2C-CA0C-4ECA-910E-021483F378D4}" type="pres">
-      <dgm:prSet presAssocID="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" presName="hierChild7" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{893ADF4F-EA23-4873-85C3-538E613FDA61}" type="pres">
@@ -9821,7 +9826,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{FDCECD47-9280-45E0-85CE-D2A95997FD1A}" type="pres">
-      <dgm:prSet presAssocID="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" presName="rootText1" presStyleLbl="node0" presStyleIdx="2" presStyleCnt="3">
+      <dgm:prSet presAssocID="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" presName="rootText1" presStyleLbl="node0" presStyleIdx="1" presStyleCnt="2">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -9829,7 +9834,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{C8165A6E-4CDA-4B21-8CB9-B5A1883C294F}" type="pres">
-      <dgm:prSet presAssocID="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" presName="rootConnector1" presStyleLbl="asst0" presStyleIdx="1" presStyleCnt="3"/>
+      <dgm:prSet presAssocID="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" presName="rootConnector1" presStyleLbl="asst0" presStyleIdx="0" presStyleCnt="2"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{4739EDB2-ADB4-415A-89E5-AE845E6B3134}" type="pres">
@@ -9841,7 +9846,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{D9974885-92EE-42A5-894E-E98575038686}" type="pres">
-      <dgm:prSet presAssocID="{0DD7BE4B-979D-45EC-88EE-602AD46EE808}" presName="Name111" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="3"/>
+      <dgm:prSet presAssocID="{0DD7BE4B-979D-45EC-88EE-602AD46EE808}" presName="Name111" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="2"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{CC388E06-708E-403A-8BD0-6A3799F9C05E}" type="pres">
@@ -9857,7 +9862,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{74E7A8D6-18BE-40E9-87FD-51164B79C2A5}" type="pres">
-      <dgm:prSet presAssocID="{279FD639-269A-4A23-83FE-90F23A7264AC}" presName="rootText3" presStyleLbl="asst0" presStyleIdx="2" presStyleCnt="3">
+      <dgm:prSet presAssocID="{279FD639-269A-4A23-83FE-90F23A7264AC}" presName="rootText3" presStyleLbl="asst0" presStyleIdx="1" presStyleCnt="2">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -9865,7 +9870,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{23B3FC26-CB2E-4E1D-B239-2A9B1DBA5F7B}" type="pres">
-      <dgm:prSet presAssocID="{279FD639-269A-4A23-83FE-90F23A7264AC}" presName="rootConnector3" presStyleLbl="asst0" presStyleIdx="2" presStyleCnt="3"/>
+      <dgm:prSet presAssocID="{279FD639-269A-4A23-83FE-90F23A7264AC}" presName="rootConnector3" presStyleLbl="asst0" presStyleIdx="1" presStyleCnt="2"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{13447806-1B61-4408-BD31-89535CC27B4F}" type="pres">
@@ -9878,24 +9883,17 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
-    <dgm:cxn modelId="{CC03E217-0E2A-47AF-87B9-B97163093591}" type="presOf" srcId="{97A0BEBB-D5A9-4338-BDDC-BB6757A5DA75}" destId="{758BB659-965A-451E-B239-65B733991407}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{D6B8891C-5ABA-4611-AF88-E4AD84CF5053}" srcId="{DD8FE056-FF76-4EFC-B4CB-C8196AED4707}" destId="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" srcOrd="1" destOrd="0" parTransId="{2AA4CF4B-BF09-48D5-A141-23C39086599F}" sibTransId="{FA3856B3-B1DD-48FB-8F49-43F2C8D53F0D}"/>
     <dgm:cxn modelId="{FF3FEA2E-F884-4B66-B1BB-1A48A3390AA6}" type="presOf" srcId="{9439E707-2878-455D-93F3-E63F2486DDE0}" destId="{AF7FB488-574D-4E27-9A8E-92293D2D553D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{170AEB47-9EA9-406C-A14A-63EBA18F0B60}" srcId="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" destId="{9439E707-2878-455D-93F3-E63F2486DDE0}" srcOrd="0" destOrd="0" parTransId="{3F3288E7-6B47-4EB6-917A-860E6A2B7D52}" sibTransId="{C6335AA2-590A-4C67-86E5-3EA4B7D8771A}"/>
     <dgm:cxn modelId="{C2FAA848-90B5-402F-B5F4-CD0FCDE7972F}" type="presOf" srcId="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" destId="{57FE20FB-F5E0-4DA2-9D76-4A2A6628A15A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{78ED1A57-A233-43E1-9B2A-12F903ECDB96}" type="presOf" srcId="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" destId="{0B0179FF-84DE-48B2-A7B2-7647C4DEF74C}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{028F1E63-9581-447D-8856-159B421903B2}" type="presOf" srcId="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" destId="{76AD2B5F-A78D-4688-A301-5DE4286FAF14}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{9AB1F770-95DD-4B28-82D9-B654329EA9B8}" type="presOf" srcId="{279FD639-269A-4A23-83FE-90F23A7264AC}" destId="{23B3FC26-CB2E-4E1D-B239-2A9B1DBA5F7B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{15219378-EA60-49D1-863A-2F106AB24A29}" type="presOf" srcId="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" destId="{FDCECD47-9280-45E0-85CE-D2A95997FD1A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{515E6081-4271-46DA-B21A-8055F973A7E6}" type="presOf" srcId="{9439E707-2878-455D-93F3-E63F2486DDE0}" destId="{4B2205FC-4A1F-4EBD-AC56-8E8D946DFC3B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{940E5F85-56DE-4443-B3A7-A33B7E4B5568}" type="presOf" srcId="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" destId="{843CB9D4-FFDE-40CB-BDF4-1B14FA03BEEE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{31CDC28C-50B9-46B8-91B6-CE93A8E85FF9}" srcId="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" destId="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" srcOrd="0" destOrd="0" parTransId="{97A0BEBB-D5A9-4338-BDDC-BB6757A5DA75}" sibTransId="{28F7DDC4-D7CA-4BF1-848F-D5B1B6F067CB}"/>
     <dgm:cxn modelId="{C474A496-199B-4366-B95E-68EE73E2E11A}" type="presOf" srcId="{0DD7BE4B-979D-45EC-88EE-602AD46EE808}" destId="{D9974885-92EE-42A5-894E-E98575038686}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{D87C8F9E-8319-4D6C-A5B5-477C2B3A91EB}" srcId="{DD8FE056-FF76-4EFC-B4CB-C8196AED4707}" destId="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" srcOrd="2" destOrd="0" parTransId="{9F30327B-5D26-4586-A496-3E5F3F41249F}" sibTransId="{20F636CE-7126-40D2-9A48-9FA2C74A8B48}"/>
-    <dgm:cxn modelId="{A45763A2-91F7-45A6-BE13-4AD253876B2A}" type="presOf" srcId="{7EDFBA5D-94DE-4FB8-BF7C-7FF93F7A1C44}" destId="{277E8B4D-5DAC-4C00-95B2-6E5ADFBAA0BC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{D87C8F9E-8319-4D6C-A5B5-477C2B3A91EB}" srcId="{DD8FE056-FF76-4EFC-B4CB-C8196AED4707}" destId="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" srcOrd="1" destOrd="0" parTransId="{9F30327B-5D26-4586-A496-3E5F3F41249F}" sibTransId="{20F636CE-7126-40D2-9A48-9FA2C74A8B48}"/>
     <dgm:cxn modelId="{A62957A4-8D40-4162-BBD3-880445B1398A}" type="presOf" srcId="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" destId="{C8165A6E-4CDA-4B21-8CB9-B5A1883C294F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{716992AE-20F6-45A4-A7FD-6F8B3031A878}" type="presOf" srcId="{3F3288E7-6B47-4EB6-917A-860E6A2B7D52}" destId="{72416332-1284-4FEA-973A-34B4871CCC3F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{B75E3EB2-C23D-4383-A575-A68E2B9FA91D}" type="presOf" srcId="{75EF91A3-91CC-417B-9749-C134CEFDE40A}" destId="{742B2A4B-0C31-45FA-A574-C4B63CA27F49}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{2C4E5FC4-4F39-485A-9605-FCCA601BFFAC}" type="presOf" srcId="{DD8FE056-FF76-4EFC-B4CB-C8196AED4707}" destId="{0F260D2F-6143-4685-82D4-B666DE6BEC5E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{A403D5CE-6600-4597-8B62-30A182D01FD5}" srcId="{DD8FE056-FF76-4EFC-B4CB-C8196AED4707}" destId="{03242B5D-4AD4-4304-B2A0-C146ACF04DA6}" srcOrd="0" destOrd="0" parTransId="{15D2CF99-A2B9-418C-A563-4BA672D4EC74}" sibTransId="{FB661218-E898-466B-A96A-8A3EB830EA43}"/>
     <dgm:cxn modelId="{1EB2A6D3-15A7-4CAB-9457-CA71C5162736}" srcId="{5B2A74B1-66A2-4062-B6D1-0A9A0476D31C}" destId="{279FD639-269A-4A23-83FE-90F23A7264AC}" srcOrd="0" destOrd="0" parTransId="{0DD7BE4B-979D-45EC-88EE-602AD46EE808}" sibTransId="{231E0303-0AC2-43E0-B5AE-20379EAF445C}"/>
@@ -9913,20 +9911,7 @@
     <dgm:cxn modelId="{B7BA294D-0E90-4404-85AD-F046B28131D3}" type="presParOf" srcId="{AB3D651E-D38A-497C-A532-965CD091AD74}" destId="{4B2205FC-4A1F-4EBD-AC56-8E8D946DFC3B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{D4BAEEDC-E04B-460D-833D-D56E4131369A}" type="presParOf" srcId="{6214A9CC-647A-4E83-9BFC-93AAA1510EFC}" destId="{2994D162-FD3E-4980-90DB-B1833056775E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{F1705082-97DD-42EE-A9BA-743CF45B14B0}" type="presParOf" srcId="{6214A9CC-647A-4E83-9BFC-93AAA1510EFC}" destId="{F367418B-F286-440A-9A7B-2BDEEDA71E8B}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{B5AEF67D-981F-4D0F-A955-9697ED71B59D}" type="presParOf" srcId="{0F260D2F-6143-4685-82D4-B666DE6BEC5E}" destId="{D6E38978-9D05-4C1C-BEFF-EF82F634E34B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{83F9DE79-C14B-4ACC-8C4F-BFCBD23CCDC5}" type="presParOf" srcId="{D6E38978-9D05-4C1C-BEFF-EF82F634E34B}" destId="{178DCAA2-D7AA-4AE4-8110-84AE55DAFB4C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7D96202C-8AAE-4994-8739-30E44F3D9A5C}" type="presParOf" srcId="{178DCAA2-D7AA-4AE4-8110-84AE55DAFB4C}" destId="{76AD2B5F-A78D-4688-A301-5DE4286FAF14}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{7EDF3419-7E5C-4806-A406-3449790B9B9E}" type="presParOf" srcId="{178DCAA2-D7AA-4AE4-8110-84AE55DAFB4C}" destId="{277E8B4D-5DAC-4C00-95B2-6E5ADFBAA0BC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{AD86FA36-93C6-47BB-AF76-233733203BCB}" type="presParOf" srcId="{D6E38978-9D05-4C1C-BEFF-EF82F634E34B}" destId="{BC4D512F-D5D5-4EC4-AB91-99C49864A5DC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{3CC78185-ECE5-44C0-8D18-3283C6401F6F}" type="presParOf" srcId="{D6E38978-9D05-4C1C-BEFF-EF82F634E34B}" destId="{8A58ACB5-52B2-4818-B571-1DE60B545CAF}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{C72AFE7B-D155-4909-99BE-B0E260530090}" type="presParOf" srcId="{8A58ACB5-52B2-4818-B571-1DE60B545CAF}" destId="{758BB659-965A-451E-B239-65B733991407}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{1BAF5298-0C45-4278-A579-CFA3BDA8674E}" type="presParOf" srcId="{8A58ACB5-52B2-4818-B571-1DE60B545CAF}" destId="{3AE659BE-DB29-4625-8029-1B3242160EB5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{02D534F1-F10D-4B1C-8831-197B4BC55B37}" type="presParOf" srcId="{3AE659BE-DB29-4625-8029-1B3242160EB5}" destId="{3B733DE7-3A47-4186-87B5-A06E7664D23B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{6212166A-3B86-43B8-9179-AEB7A5F277BF}" type="presParOf" srcId="{3B733DE7-3A47-4186-87B5-A06E7664D23B}" destId="{843CB9D4-FFDE-40CB-BDF4-1B14FA03BEEE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{C0133E69-C075-4EF0-B5AC-B098DCEB990F}" type="presParOf" srcId="{3B733DE7-3A47-4186-87B5-A06E7664D23B}" destId="{742B2A4B-0C31-45FA-A574-C4B63CA27F49}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{069A2F98-E601-41FB-8094-1CFDC3B66A07}" type="presParOf" srcId="{3AE659BE-DB29-4625-8029-1B3242160EB5}" destId="{F3383217-A95D-4C77-B90E-4D8D3300A368}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{88FC9DDC-9BD4-4E90-8655-9F911E1E61BB}" type="presParOf" srcId="{3AE659BE-DB29-4625-8029-1B3242160EB5}" destId="{473CAF2C-CA0C-4ECA-910E-021483F378D4}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{5B92C0EE-B470-436D-B951-556E622FA544}" type="presParOf" srcId="{0F260D2F-6143-4685-82D4-B666DE6BEC5E}" destId="{893ADF4F-EA23-4873-85C3-538E613FDA61}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{5B92C0EE-B470-436D-B951-556E622FA544}" type="presParOf" srcId="{0F260D2F-6143-4685-82D4-B666DE6BEC5E}" destId="{893ADF4F-EA23-4873-85C3-538E613FDA61}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{4C2B4F75-D0DD-4188-A981-D1B461EC1569}" type="presParOf" srcId="{893ADF4F-EA23-4873-85C3-538E613FDA61}" destId="{8E8DFC8E-0955-4C95-B369-56258DFC686C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{3F0A92B6-52A6-4E0D-AB11-91F61C0143B4}" type="presParOf" srcId="{8E8DFC8E-0955-4C95-B369-56258DFC686C}" destId="{FDCECD47-9280-45E0-85CE-D2A95997FD1A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{D7843117-F3A5-468A-B400-E93100008C58}" type="presParOf" srcId="{8E8DFC8E-0955-4C95-B369-56258DFC686C}" destId="{C8165A6E-4CDA-4B21-8CB9-B5A1883C294F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
@@ -14629,8 +14614,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3133438" y="2994062"/>
-          <a:ext cx="416184" cy="91440"/>
+          <a:off x="3124512" y="3345949"/>
+          <a:ext cx="404473" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14644,7 +14629,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="416184" y="45720"/>
+                <a:pt x="404473" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14699,8 +14684,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3331125" y="3029377"/>
-        <a:ext cx="20809" cy="20809"/>
+        <a:off x="3316637" y="3381557"/>
+        <a:ext cx="20223" cy="20223"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{77676E43-8DE8-4B80-A2D5-144E37F4A310}">
@@ -14710,8 +14695,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="636333" y="1850231"/>
-          <a:ext cx="416184" cy="1189550"/>
+          <a:off x="697672" y="1850231"/>
+          <a:ext cx="404473" cy="1541437"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14725,13 +14710,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="208092" y="0"/>
+                <a:pt x="202236" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="208092" y="1189550"/>
+                <a:pt x="202236" y="1541437"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="416184" y="1189550"/>
+                <a:pt x="404473" y="1541437"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14786,8 +14771,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="812919" y="2413500"/>
-        <a:ext cx="63012" cy="63012"/>
+        <a:off x="860068" y="2581109"/>
+        <a:ext cx="79681" cy="79681"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{584ACE3F-ACE1-4261-AE80-2CB0DB735E28}">
@@ -14797,8 +14782,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3133438" y="2201028"/>
-          <a:ext cx="416184" cy="91440"/>
+          <a:off x="3124512" y="2575230"/>
+          <a:ext cx="404473" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14812,7 +14797,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="416184" y="45720"/>
+                <a:pt x="404473" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14867,8 +14852,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3331125" y="2236343"/>
-        <a:ext cx="20809" cy="20809"/>
+        <a:off x="3316637" y="2610838"/>
+        <a:ext cx="20223" cy="20223"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F60EF4BE-E262-410F-8D97-2339F1312225}">
@@ -14878,8 +14863,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="636333" y="1850231"/>
-          <a:ext cx="416184" cy="396516"/>
+          <a:off x="697672" y="1850231"/>
+          <a:ext cx="404473" cy="770718"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14893,13 +14878,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="208092" y="0"/>
+                <a:pt x="202236" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="208092" y="396516"/>
+                <a:pt x="202236" y="770718"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="416184" y="396516"/>
+                <a:pt x="404473" y="770718"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -14954,19 +14939,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="830054" y="2034119"/>
-        <a:ext cx="28741" cy="28741"/>
+        <a:off x="878149" y="2213830"/>
+        <a:ext cx="43520" cy="43520"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{7BE09262-5205-4BA1-8F1F-55ACC71B1C56}">
+    <dsp:sp modelId="{B90C310D-D549-524B-987B-D38E9BFADBD2}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3133438" y="1407994"/>
-          <a:ext cx="416184" cy="91440"/>
+          <a:off x="3124512" y="1804511"/>
+          <a:ext cx="404473" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14980,7 +14965,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="416184" y="45720"/>
+                <a:pt x="404473" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15035,19 +15020,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3331125" y="1443309"/>
-        <a:ext cx="20809" cy="20809"/>
+        <a:off x="3316637" y="1840119"/>
+        <a:ext cx="20223" cy="20223"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{DEDE2411-A30D-4A55-809B-43C5A22D7862}">
+    <dsp:sp modelId="{45E60197-1614-F24B-9940-ADF896B04C94}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="636333" y="1453714"/>
-          <a:ext cx="416184" cy="396516"/>
+          <a:off x="697672" y="1804511"/>
+          <a:ext cx="404473" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -15058,16 +15043,178 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="396516"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="208092" y="396516"/>
+                <a:pt x="404473" y="45720"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="889797" y="1840119"/>
+        <a:ext cx="20223" cy="20223"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3093995" y="1033792"/>
+          <a:ext cx="434990" cy="91440"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="45720"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="434990" y="45720"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3300615" y="1068637"/>
+        <a:ext cx="21749" cy="21749"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{57864B81-8F04-4470-9267-28EB35714A78}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="697672" y="1079512"/>
+          <a:ext cx="373955" cy="770718"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="770718"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="186977" y="770718"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="208092" y="0"/>
+                <a:pt x="186977" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="416184" y="0"/>
+                <a:pt x="373955" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15122,19 +15269,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="830054" y="1637602"/>
-        <a:ext cx="28741" cy="28741"/>
+        <a:off x="863234" y="1443455"/>
+        <a:ext cx="42832" cy="42832"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{9F3627B0-9A84-4EC2-9ACF-C54F857716E3}">
+    <dsp:sp modelId="{F5B07602-6216-104D-881E-C22D3FD7B48A}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3102037" y="614960"/>
-          <a:ext cx="447585" cy="91440"/>
+          <a:off x="3124512" y="263073"/>
+          <a:ext cx="404473" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -15148,7 +15295,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="447585" y="45720"/>
+                <a:pt x="404473" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15199,23 +15346,23 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="500" kern="1200"/>
+          <a:endParaRPr lang="en-GB" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3314640" y="649491"/>
-        <a:ext cx="22379" cy="22379"/>
+        <a:off x="3316637" y="298681"/>
+        <a:ext cx="20223" cy="20223"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{57864B81-8F04-4470-9267-28EB35714A78}">
+    <dsp:sp modelId="{91EBC5E0-9F71-7D43-BF83-38911486F0BD}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="636333" y="660680"/>
-          <a:ext cx="384783" cy="1189550"/>
+          <a:off x="697672" y="308793"/>
+          <a:ext cx="404473" cy="1541437"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -15226,16 +15373,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="1189550"/>
+                <a:pt x="0" y="1541437"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="192391" y="1189550"/>
+                <a:pt x="202236" y="1541437"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="192391" y="0"/>
+                <a:pt x="202236" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="384783" y="0"/>
+                <a:pt x="404473" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -15286,12 +15433,12 @@
             </a:spcAft>
             <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="500" kern="1200"/>
+          <a:endParaRPr lang="en-GB" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="797469" y="1224200"/>
-        <a:ext cx="62511" cy="62511"/>
+        <a:off x="860068" y="1039671"/>
+        <a:ext cx="79681" cy="79681"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{AD3CFF9F-AEA2-4310-ADA7-A0F0768158A7}">
@@ -15301,8 +15448,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="-1350424" y="1533017"/>
-          <a:ext cx="3339089" cy="634427"/>
+          <a:off x="-1233181" y="1541943"/>
+          <a:ext cx="3245132" cy="616575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15344,12 +15491,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="26035" tIns="26035" rIns="26035" bIns="26035" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="25400" tIns="25400" rIns="25400" bIns="25400" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1822450">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1778000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -15362,14 +15509,188 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="4100" kern="1200"/>
+            <a:rPr lang="en-US" sz="4000" kern="1200"/>
             <a:t>Cash flow</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="-1350424" y="1533017"/>
-        <a:ext cx="3339089" cy="634427"/>
+        <a:off x="-1233181" y="1541943"/>
+        <a:ext cx="3245132" cy="616575"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{BBE1A5C2-FD17-294F-A528-E8FBBB038CC3}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1102145" y="505"/>
+          <a:ext cx="2022366" cy="616575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200"/>
+            <a:t>Income - expense &lt; monthly payment</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="1102145" y="505"/>
+        <a:ext cx="2022366" cy="616575"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{4F8902AC-2B83-1046-AEA2-477D6C7D476B}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3528985" y="505"/>
+          <a:ext cx="2022366" cy="616575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" kern="1200"/>
+            <a:t>Score - 10</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" kern="1200"/>
+            <a:t>Interest rate -.-5</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3528985" y="505"/>
+        <a:ext cx="2022366" cy="616575"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{3FD72082-2FD5-45DA-A0E1-0AEFDB83D3FA}">
@@ -15379,8 +15700,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1021116" y="343467"/>
-          <a:ext cx="2080920" cy="634427"/>
+          <a:off x="1071628" y="771224"/>
+          <a:ext cx="2022366" cy="616575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15446,8 +15767,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1021116" y="343467"/>
-        <a:ext cx="2080920" cy="634427"/>
+        <a:off x="1071628" y="771224"/>
+        <a:ext cx="2022366" cy="616575"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{762E18FB-67EB-41E4-8EBC-5D3B2348F1AE}">
@@ -15457,8 +15778,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3549622" y="343467"/>
-          <a:ext cx="2080920" cy="634427"/>
+          <a:off x="3528985" y="771224"/>
+          <a:ext cx="2022366" cy="616575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15542,19 +15863,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3549622" y="343467"/>
-        <a:ext cx="2080920" cy="634427"/>
+        <a:off x="3528985" y="771224"/>
+        <a:ext cx="2022366" cy="616575"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{59A5A8BE-646D-4A35-AB72-C89F408C38C1}">
+    <dsp:sp modelId="{370868FA-82A6-F84C-B5AC-0762E5864E9B}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1052517" y="1136501"/>
-          <a:ext cx="2080920" cy="634427"/>
+          <a:off x="1102145" y="1541943"/>
+          <a:ext cx="2022366" cy="616575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15615,24 +15936,25 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400" kern="1200"/>
-            <a:t>Remainder after expenses more than the monthly repayment of the loan*2 </a:t>
+            <a:t>income - expense &gt; monthly repayment of the loan*2 </a:t>
           </a:r>
+          <a:endParaRPr lang="en-GB" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1052517" y="1136501"/>
-        <a:ext cx="2080920" cy="634427"/>
+        <a:off x="1102145" y="1541943"/>
+        <a:ext cx="2022366" cy="616575"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{095E95D6-0B9B-4DD2-B0A7-02C8F3D83AEE}">
+    <dsp:sp modelId="{8AB46E28-35C3-7C44-919A-064D9B12A93B}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3549622" y="1136501"/>
-          <a:ext cx="2080920" cy="634427"/>
+          <a:off x="3528985" y="1541943"/>
+          <a:ext cx="2022366" cy="616575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15711,13 +16033,13 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400" kern="1200"/>
-            <a:t>Interes rate 0.01</a:t>
+            <a:t>Interest rate 0.01</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3549622" y="1136501"/>
-        <a:ext cx="2080920" cy="634427"/>
+        <a:off x="3528985" y="1541943"/>
+        <a:ext cx="2022366" cy="616575"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{606CCE1F-A7DB-4848-9758-D76A1652749D}">
@@ -15727,8 +16049,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1052517" y="1929534"/>
-          <a:ext cx="2080920" cy="634427"/>
+          <a:off x="1102145" y="2312662"/>
+          <a:ext cx="2022366" cy="616575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15789,13 +16111,13 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400" kern="1200"/>
-            <a:t>Remainder after expenses more or equal to monthly repayment of the loan*1.5</a:t>
+            <a:t>income - expense &gt; monthly repayment of the loan*1.5</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1052517" y="1929534"/>
-        <a:ext cx="2080920" cy="634427"/>
+        <a:off x="1102145" y="2312662"/>
+        <a:ext cx="2022366" cy="616575"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{996D80AD-81CA-4696-85B7-0E13A7FFDEC7}">
@@ -15805,8 +16127,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3549622" y="1929534"/>
-          <a:ext cx="2080920" cy="634427"/>
+          <a:off x="3528985" y="2312662"/>
+          <a:ext cx="2022366" cy="616575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15890,8 +16212,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3549622" y="1929534"/>
-        <a:ext cx="2080920" cy="634427"/>
+        <a:off x="3528985" y="2312662"/>
+        <a:ext cx="2022366" cy="616575"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E82C79BE-4890-4781-B4F6-B9DDEEBD6944}">
@@ -15901,8 +16223,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1052517" y="2722568"/>
-          <a:ext cx="2080920" cy="634427"/>
+          <a:off x="1102145" y="3083381"/>
+          <a:ext cx="2022366" cy="616575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15963,13 +16285,13 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400" kern="1200"/>
-            <a:t>Remainder after expenses less or equal to monthly repayment of the loan</a:t>
+            <a:t>income - expense &gt;= monthly repayment of the loan</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1052517" y="2722568"/>
-        <a:ext cx="2080920" cy="634427"/>
+        <a:off x="1102145" y="3083381"/>
+        <a:ext cx="2022366" cy="616575"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{43EC8F67-419F-4097-95A1-42F22F604BF1}">
@@ -15979,8 +16301,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3549622" y="2722568"/>
-          <a:ext cx="2080920" cy="634427"/>
+          <a:off x="3528985" y="3083381"/>
+          <a:ext cx="2022366" cy="616575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16064,8 +16386,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3549622" y="2722568"/>
-        <a:ext cx="2080920" cy="634427"/>
+        <a:off x="3528985" y="3083381"/>
+        <a:ext cx="2022366" cy="616575"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -16815,7 +17137,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1800" kern="1200"/>
-            <a:t>Score -100</a:t>
+            <a:t>Score -120</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
@@ -16843,8 +17165,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6234181" y="1539784"/>
-          <a:ext cx="191384" cy="838447"/>
+          <a:off x="5760376" y="1457493"/>
+          <a:ext cx="273675" cy="1198959"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -16855,72 +17177,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="191384" y="0"/>
+                <a:pt x="273675" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="191384" y="838447"/>
+                <a:pt x="273675" y="1198959"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="838447"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{758BB659-965A-451E-B239-65B733991407}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4028698" y="1539784"/>
-          <a:ext cx="191384" cy="838447"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="191384" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="191384" y="838447"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="838447"/>
+                <a:pt x="0" y="1198959"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -16961,8 +17224,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1823216" y="1539784"/>
-          <a:ext cx="191384" cy="838447"/>
+          <a:off x="2606591" y="1457493"/>
+          <a:ext cx="273675" cy="1198959"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -16973,13 +17236,13 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="191384" y="0"/>
+                <a:pt x="273675" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="191384" y="838447"/>
+                <a:pt x="273675" y="1198959"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="838447"/>
+                <a:pt x="0" y="1198959"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -17020,8 +17283,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1103244" y="628427"/>
-          <a:ext cx="1822712" cy="911356"/>
+          <a:off x="1577049" y="154276"/>
+          <a:ext cx="2606434" cy="1303217"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17063,12 +17326,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="19685" tIns="19685" rIns="19685" bIns="19685" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="27940" rIns="27940" bIns="27940" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1377950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1955800">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -17081,14 +17344,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="3100" kern="1200"/>
-            <a:t>Over 90</a:t>
+            <a:rPr lang="en-US" sz="4400" kern="1200"/>
+            <a:t>Score &gt;= 70</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1103244" y="628427"/>
-        <a:ext cx="1822712" cy="911356"/>
+        <a:off x="1577049" y="154276"/>
+        <a:ext cx="2606434" cy="1303217"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{AF7FB488-574D-4E27-9A8E-92293D2D553D}">
@@ -17098,8 +17361,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="503" y="1922553"/>
-          <a:ext cx="1822712" cy="911356"/>
+          <a:off x="156" y="2004844"/>
+          <a:ext cx="2606434" cy="1303217"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17141,12 +17404,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="19685" tIns="19685" rIns="19685" bIns="19685" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="27940" rIns="27940" bIns="27940" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1377950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1955800">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -17159,25 +17422,25 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="3100" kern="1200"/>
+            <a:rPr lang="en-US" sz="4400" kern="1200"/>
             <a:t>Approved </a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="503" y="1922553"/>
-        <a:ext cx="1822712" cy="911356"/>
+        <a:off x="156" y="2004844"/>
+        <a:ext cx="2606434" cy="1303217"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{76AD2B5F-A78D-4688-A301-5DE4286FAF14}">
+    <dsp:sp modelId="{FDCECD47-9280-45E0-85CE-D2A95997FD1A}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3308727" y="628427"/>
-          <a:ext cx="1822712" cy="911356"/>
+          <a:off x="4730834" y="154276"/>
+          <a:ext cx="2606434" cy="1303217"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17219,12 +17482,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="19685" tIns="19685" rIns="19685" bIns="19685" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="27940" rIns="27940" bIns="27940" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1377950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1955800">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -17237,25 +17500,25 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="3100" kern="1200"/>
-            <a:t>Between 50 - 90</a:t>
+            <a:rPr lang="en-US" sz="4400" kern="1200"/>
+            <a:t>Score &lt; 70</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3308727" y="628427"/>
-        <a:ext cx="1822712" cy="911356"/>
+        <a:off x="4730834" y="154276"/>
+        <a:ext cx="2606434" cy="1303217"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{843CB9D4-FFDE-40CB-BDF4-1B14FA03BEEE}">
+    <dsp:sp modelId="{74E7A8D6-18BE-40E9-87FD-51164B79C2A5}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2205986" y="1922553"/>
-          <a:ext cx="1822712" cy="911356"/>
+          <a:off x="3153942" y="2004844"/>
+          <a:ext cx="2606434" cy="1303217"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17297,12 +17560,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="19685" tIns="19685" rIns="19685" bIns="19685" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="27940" tIns="27940" rIns="27940" bIns="27940" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1377950">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1955800">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -17315,170 +17578,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="3100" kern="1200"/>
-            <a:t>Approved</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2205986" y="1922553"/>
-        <a:ext cx="1822712" cy="911356"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{FDCECD47-9280-45E0-85CE-D2A95997FD1A}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5514209" y="628427"/>
-          <a:ext cx="1822712" cy="911356"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="19685" tIns="19685" rIns="19685" bIns="19685" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1377950">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="3100" kern="1200"/>
-            <a:t>Under 50</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="5514209" y="628427"/>
-        <a:ext cx="1822712" cy="911356"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{74E7A8D6-18BE-40E9-87FD-51164B79C2A5}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4411468" y="1922553"/>
-          <a:ext cx="1822712" cy="911356"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="19685" tIns="19685" rIns="19685" bIns="19685" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1377950">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="3100" kern="1200"/>
+            <a:rPr lang="en-US" sz="4400" kern="1200"/>
             <a:t>Rejected</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4411468" y="1922553"/>
-        <a:ext cx="1822712" cy="911356"/>
+        <a:off x="3153942" y="2004844"/>
+        <a:ext cx="2606434" cy="1303217"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -29373,8 +29480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L27" workbookViewId="0">
-      <selection activeCell="AE40" sqref="AE40"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>